<commit_message>
Correction Made in carrier count
</commit_message>
<xml_diff>
--- a/ICMS_EP2/data/testdata.xlsx
+++ b/ICMS_EP2/data/testdata.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>433938</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>433982</t>
+  </si>
+  <si>
+    <t>433986</t>
   </si>
 </sst>
 </file>
@@ -505,7 +508,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implemented validation for Invalid user
</commit_message>
<xml_diff>
--- a/ICMS_EP2/data/testdata.xlsx
+++ b/ICMS_EP2/data/testdata.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>433938</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>433986</t>
+  </si>
+  <si>
+    <t>433988</t>
   </si>
 </sst>
 </file>
@@ -508,7 +511,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25"/>

</xml_diff>